<commit_message>
log To Console with log4j
</commit_message>
<xml_diff>
--- a/Inputsheets/Data.xlsx
+++ b/Inputsheets/Data.xlsx
@@ -3,15 +3,19 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{3B404655-68FD-49B7-A553-CFD9A84C087D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gourave\workspace\TestProject\Inputsheets\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24460F2A-50D0-4527-BBDA-DD553AA629E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="20670" windowHeight="11700" xr2:uid="{3CF02EC1-67D5-4B91-A7C4-A3AE21B76A86}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{3CF02EC1-67D5-4B91-A7C4-A3AE21B76A86}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Username</t>
   </si>
@@ -39,6 +43,12 @@
   </si>
   <si>
     <t>Test Value</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com</t>
+  </si>
+  <si>
+    <t>URL</t>
   </si>
 </sst>
 </file>
@@ -100,7 +110,9 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,14 +427,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60B67613-8DCC-41B5-AB8C-401E2742D6D7}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -449,6 +463,46 @@
         <v>3</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>